<commit_message>
Aggiornato file dei risultati dei test
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#180913000000XX/aopc/repo-aopc/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#180913000000XX/aopc/repo-aopc/1.0.0/report-checklist.xlsx
@@ -1942,11 +1942,11 @@
   <dimension ref="A1:U671"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
+      <selection pane="bottomRight" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>